<commit_message>
V1_update sql and diagram
</commit_message>
<xml_diff>
--- a/00_DataShare/ChiaViecNhom.xlsx
+++ b/00_DataShare/ChiaViecNhom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\btck_Shopqa\00_DataShare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0465AFC5-1F98-4159-B10A-F7E161324664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7298088D-6E13-47F2-9F08-1D427E8DE0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>No#</t>
   </si>
@@ -221,12 +221,15 @@
     <t>Dự trên thông tin khách hàng, Số đo, chiều cao cân nặng, đề xuât sản phẩm phù hợp
 Hoặc dựa trên màu sắc sở thik đề xuất sản phẩm phù hợp</t>
   </si>
+  <si>
+    <t>Thanh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,13 +243,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -261,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -275,6 +291,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,40 +677,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.3984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="52.3984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.19921875" customWidth="1"/>
+    <col min="3" max="3" width="21.19921875" style="5" customWidth="1"/>
     <col min="4" max="5" width="12.3984375" customWidth="1"/>
     <col min="6" max="6" width="13.59765625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -690,6 +722,12 @@
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="11">
+        <v>45778</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -698,6 +736,9 @@
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="E4" s="10">
+        <v>45782</v>
+      </c>
       <c r="G4" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -709,6 +750,9 @@
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="E5" s="10">
+        <v>45782</v>
+      </c>
       <c r="G5" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -720,6 +764,9 @@
       <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="E6" s="10">
+        <v>45782</v>
+      </c>
       <c r="G6" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
@@ -731,6 +778,9 @@
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="E7" s="10">
+        <v>45782</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -739,6 +789,9 @@
       <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="E8" s="10">
+        <v>45782</v>
+      </c>
       <c r="G8" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
@@ -750,6 +803,9 @@
       <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="E9" s="10">
+        <v>45782</v>
+      </c>
       <c r="G9" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
@@ -761,6 +817,9 @@
       <c r="B10" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="E10" s="10">
+        <v>45782</v>
+      </c>
       <c r="G10" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
@@ -772,6 +831,9 @@
       <c r="B11" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="E11" s="10">
+        <v>45782</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -780,6 +842,9 @@
       <c r="B12" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E12" s="10">
+        <v>45782</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -787,6 +852,9 @@
       </c>
       <c r="B13" s="4" t="s">
         <v>35</v>
+      </c>
+      <c r="E13" s="10">
+        <v>45782</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>